<commit_message>
tercer enemy pt 1
</commit_message>
<xml_diff>
--- a/EnemyStats.xlsx
+++ b/EnemyStats.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>HitPoints</t>
   </si>
@@ -31,6 +29,9 @@
   </si>
   <si>
     <t>BP_EnemyGoblin</t>
+  </si>
+  <si>
+    <t>BP_EnemySoldier</t>
   </si>
 </sst>
 </file>
@@ -369,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -399,13 +400,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="C2">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="D2">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -413,40 +414,30 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C3">
-        <v>300</v>
+        <v>320</v>
       </c>
       <c r="D3">
-        <v>60</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>90</v>
+      </c>
+      <c r="C4">
+        <v>180</v>
+      </c>
+      <c r="D4">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>